<commit_message>
subiendo Product Backlog corregido
</commit_message>
<xml_diff>
--- a/Product_Backlog.xlsx
+++ b/Product_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\mascotas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97EBD1C1-1411-4BBA-BA8C-6D4A6D1C2B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5004CA6-0527-4503-868E-E8D091DC8DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{58062F66-ED81-45AF-951F-DB4BCFFCDE7D}"/>
   </bookViews>
@@ -93,15 +93,9 @@
     <t>Gestión de cuentas y roles de usuario</t>
   </si>
   <si>
-    <t>Roles creados, editables, asignables a cuentas.</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
-    <t>Los usuarios pueden registrarse, iniciar sesión y tener roles definidos.</t>
-  </si>
-  <si>
     <t>Como administrador, quiero crear y asignar roles para controlar el acceso.</t>
   </si>
   <si>
@@ -111,159 +105,90 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Contraseña actualizable, último acceso registrado correctamente.</t>
-  </si>
-  <si>
     <t>Validar estados de registro activos/inactivos para cuentas y roles.</t>
   </si>
   <si>
-    <t>Solo registros activos pueden iniciar sesión o ser asignados.</t>
-  </si>
-  <si>
     <t>Gestión de clientes y sus mascotas</t>
   </si>
   <si>
-    <t>Cada cliente puede registrar sus datos y los de sus mascotas.</t>
-  </si>
-  <si>
     <t>Como cliente, quiero registrar a mis mascotas con sus características y alergias.</t>
   </si>
   <si>
-    <t>Formulario de mascota funcional con validaciones obligatorias.</t>
-  </si>
-  <si>
     <t>Como cliente, quiero agregar y actualizar mis direcciones de entrega.</t>
   </si>
   <si>
-    <t>Direcciones con latitud/longitud y opción “principal”.</t>
-  </si>
-  <si>
     <t>Como cliente, quiero ver el historial de mi mascota.</t>
   </si>
   <si>
-    <t>Historial visible por fechas y editable por el nutricionista.</t>
-  </si>
-  <si>
     <t>Gestión de productos BARF y platos combinados</t>
   </si>
   <si>
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Los productos y platos pueden crearse, combinarse y publicarse.</t>
-  </si>
-  <si>
     <t>Como nutricionista, quiero crear platos combinados con productos crudos o cocidos.</t>
   </si>
   <si>
-    <t>Permite elegir productos, cantidades y marcar “es crudo”.</t>
-  </si>
-  <si>
     <t>Como cliente, quiero ver los platos disponibles y sus descripciones.</t>
   </si>
   <si>
-    <t>Lista de platos publicados con precio, imagen y descripción.</t>
-  </si>
-  <si>
     <t>Optimizar carga de imágenes de platos y productos.</t>
   </si>
   <si>
-    <t>Carga en menos de 2 segundos promedio.</t>
-  </si>
-  <si>
     <t>Consultas y planificación de dietas</t>
   </si>
   <si>
     <t>Sprint 4</t>
   </si>
   <si>
-    <t>Permitir agendar consultas y generar dietas personalizadas.</t>
-  </si>
-  <si>
     <t>Como cliente, quiero solicitar una consulta con un nutricionista.</t>
   </si>
   <si>
-    <t>Selección de fecha, mascota y nutricionista disponibles.</t>
-  </si>
-  <si>
     <t>Como nutricionista, quiero registrar recomendaciones y dietas para cada mascota.</t>
   </si>
   <si>
-    <t>Dieta con platos, fechas, instrucciones y frecuencia.</t>
-  </si>
-  <si>
     <t>Garantizar integridad y seguridad de datos de salud animal.</t>
   </si>
   <si>
-    <t>Encriptación y validación de permisos en consultas.</t>
-  </si>
-  <si>
     <t>Flujo de pedidos, asignación y entrega</t>
   </si>
   <si>
     <t>Sprint 5</t>
   </si>
   <si>
-    <t>El cliente puede realizar pedidos y confirmar entregas.</t>
-  </si>
-  <si>
     <t>Como cliente, quiero realizar un pedido y seleccionar método de pago.</t>
   </si>
   <si>
-    <t>Pedido genera detalle y total automáticamente.</t>
-  </si>
-  <si>
     <t>Como repartidor, quiero ver mis pedidos asignados y confirmar entregas.</t>
   </si>
   <si>
-    <t>Confirmación con marca “entregado” y fecha registrada.</t>
-  </si>
-  <si>
     <t>Corregir error en cálculo del subtotal en detalle del pedido.</t>
   </si>
   <si>
     <t>Crítica</t>
   </si>
   <si>
-    <t>Subtotal correcto según cantidad y precio.</t>
-  </si>
-  <si>
     <t>Módulo de pagos y pasarelas</t>
   </si>
   <si>
     <t>Sprint 6</t>
   </si>
   <si>
-    <t>Registrar pagos y sus historiales.</t>
-  </si>
-  <si>
     <t>Como cliente, quiero pagar con diferentes métodos (QR, transferencia, tarjeta).</t>
   </si>
   <si>
-    <t>Pasarela seleccionable, monto y referencia válidos.</t>
-  </si>
-  <si>
     <t>Como administrador, quiero ver el historial de pagos y su estado.</t>
   </si>
   <si>
-    <t>Pagos listados por fecha, estado y método.</t>
-  </si>
-  <si>
     <t>Tiempos de carga menores a 2s en todo el sistema.</t>
   </si>
   <si>
     <t>Global</t>
   </si>
   <si>
-    <t>Promedio &lt; 2 segundos.</t>
-  </si>
-  <si>
     <t>Cumplir con políticas de seguridad y encriptación de contraseñas.</t>
   </si>
   <si>
-    <t>Hash seguro y política de contraseñas.</t>
-  </si>
-  <si>
     <t>Alexandra</t>
   </si>
   <si>
@@ -271,6 +196,154 @@
   </si>
   <si>
     <t>Paul</t>
+  </si>
+  <si>
+    <t>Dado que un usuario completa el formulario de registro con nombre de usuario, correo electrónico y contraseña, entonces el sistema crea un registro en Cuenta de usuario con estado de registro = activo y último acceso = null.
+Dado que un usuario inicia sesión correctamente, el sistema actualiza el campo último acceso con la fecha y hora actuales.
+Dado que un usuario tiene estado inactivo (estado de registro = 0), el sistema impide su acceso.
+Dado que un administrador consulta los usuarios, el sistema lista cuentas con su rol y estado.</t>
+  </si>
+  <si>
+    <t>Dado que un usuario accede al módulo de perfil, puede cambiar su contraseña; el sistema la encripta con bcrypt o Argon2 antes de guardarla.
+Dado que se realiza un cambio exitoso, el campo último acceso se mantiene actualizado.
+Dado que se ingresa una contraseña débil, el sistema muestra un mensaje de validación.
+Dado que el usuario guarda cambios, el sistema registra la fecha del cambio de contraseña.</t>
+  </si>
+  <si>
+    <t>Dado que un cliente se crea, se vincula a una Cuenta de usuario.
+Dado que el cliente registra su mascota, se guarda el registro con datos obligatorios (nombre, especie, sexo, edad, peso).
+Dado que se actualiza una mascota, el sistema guarda una entrada en Historial de mascota.
+Dado que una mascota está inactiva, no aparece en listados activos.</t>
+  </si>
+  <si>
+    <t>Dado que un cliente completa el formulario, el sistema valida campos requeridos.
+Dado que registra alergias o gustos, el sistema las almacena en texto dentro del campo correspondiente.
+Dado que se carga una foto, se almacena en el campo foto.
+Dado que la mascota se crea, se genera un ID único vinculado al cliente.</t>
+  </si>
+  <si>
+    <t>Dado que el administrador crea un nuevo rol con nombre y descripción, el sistema guarda el registro con estado de registro = activo.
+Dado que un rol es asignado a una cuenta de usuario, se crea un registro en Usuario rol.
+Dado que el rol es editado, se actualiza la información sin duplicar registros.
+Dado que un rol es desactivado, deja de estar disponible para asignaciones nuevas.</t>
+  </si>
+  <si>
+    <t>Dado que una cuenta tiene estado de registro = 0, el sistema bloquea su acceso.
+Dado que un rol está inactivo, no puede asignarse.
+Dado que un administrador cambia un estado, se registra el cambio con fecha y usuario responsable.</t>
+  </si>
+  <si>
+    <t>Dado que un cliente agrega una dirección, el sistema valida latitud, longitud, y marca es principal.
+Dado que se marca una dirección como principal, todas las demás cambian a es principal = 0.
+Dado que una dirección se edita, los cambios se reflejan en pedidos nuevos.
+Dado que una dirección se elimina, no puede usarse en pedidos activos.</t>
+  </si>
+  <si>
+    <t>Dado que el cliente abre el historial, el sistema lista entradas por fecha y descripción.
+Dado que un nutricionista actualiza una observación, se agrega un nuevo registro.
+Dado que se solicita exportar el historial, el sistema genera PDF.
+Dado que el usuario no tiene permiso, se bloquea la visualización.</t>
+  </si>
+  <si>
+    <t>Dado que un nutricionista crea un producto, se guarda su tipo (crudo/cocido).
+Dado que combina varios productos, el sistema genera un Plato combinado.
+Dado que se publica un plato (publicado = 1), aparece en el catálogo.
+Dado que un producto se desactiva, se excluye automáticamente de combinaciones futuras.</t>
+  </si>
+  <si>
+    <t>Dado que el nutricionista selecciona productos y cantidades, se crean relaciones en Plato producto.
+Dado que se marca “es crudo”, el sistema actualiza el campo correspondiente.
+Dado que se guarda el plato, el campo creado por nutricionista = 1.
+Dado que se publica, se cambia el estado publicado = true.</t>
+  </si>
+  <si>
+    <t>Dado que un cliente consulta el catálogo, el sistema muestra platos con publicado = 1.
+Dado que selecciona un plato, se muestran precio, imagen, descripción.
+Dado que el plato se desactiva, deja de aparecer.
+Dado que se actualiza, los cambios son visibles de inmediato.</t>
+  </si>
+  <si>
+    <t>Dado que se listan platos o productos, las imágenes cargan en menos de 2 segundos.
+Dado que una imagen supera el peso máximo, el sistema la optimiza automáticamente.
+Dado que se borra una imagen, no se rompe la vista del catálogo.
+Dado que se actualiza una imagen, se reemplaza en la nube.</t>
+  </si>
+  <si>
+    <t>Dado que el cliente solicita una consulta, el sistema valida disponibilidad del Nutricionista.
+Dado que se genera la consulta, el estado inicial es “pendiente”.
+Dado que el nutricionista la aprueba, se crea una dieta personalizada.
+Dado que la consulta se completa, cambia su estado de registro a inactiva.</t>
+  </si>
+  <si>
+    <t>Dado que el cliente selecciona una mascota, una fecha, y un nutricionista, el sistema valida disponibilidad.
+Dado que la cita se confirma, el sistema guarda observaciones y recomendaciones.
+Dado que el cliente cancela antes de 24h, se cambia a “cancelada”.
+Dado que la cita expira, el estado cambia a “finalizada”.</t>
+  </si>
+  <si>
+    <t>Dado que el nutricionista crea una dieta, debe incluir nombre, descripción, fecha de inicio.
+Dado que agrega detalles, se crean registros en Detalle de dieta con plato combinado y frecuencia.
+Dado que la dieta se guarda, el cliente puede visualizarla.
+Dado que se actualiza, la versión anterior se guarda en historial.</t>
+  </si>
+  <si>
+    <t>Dado que se accede a datos de salud, solo usuarios autorizados pueden leerlos.
+Dado que se almacenan, se encriptan en tránsito y en reposo.
+Dado que ocurre un intento no autorizado, se genera un log.
+Dado que se eliminan datos, se anonimiza la información sensible</t>
+  </si>
+  <si>
+    <t>Dado que el cliente genera un pedido, se crea registro con total y método de pago.
+Dado que el repartidor confirma entrega, se guarda confirmación de entrega = true.
+Dado que se actualiza un pedido, el sistema mantiene el historial.
+Dado que un pedido finaliza, cambia su estado a “entregado”.</t>
+  </si>
+  <si>
+    <t>Dado que el cliente selecciona productos, el sistema calcula subtotal y total.
+Dado que elige método de pago, este se guarda en el campo correspondiente.
+Dado que se confirma el pedido, se genera notificación.
+Dado que el pedido está pagado, se marca como “procesado”.</t>
+  </si>
+  <si>
+    <t>Dado que el repartidor inicia sesión, ve sus pedidos asignados.
+Dado que confirma una entrega, se guarda fecha de entrega y confirmación de entrega = true.
+Dado que marca entrega, el cliente recibe notificación.
+Dado que un pedido está en tránsito, el estado refleja “en camino”.</t>
+  </si>
+  <si>
+    <t>Dado que se agrega un plato, el sistema calcula subtotal = cantidad * precio.
+Dado que se elimina un ítem, el subtotal se recalcula.
+Dado que se guarda un pedido, los valores coinciden con la base de datos.
+Dado que el total cambia, se actualiza automáticamente en Pedido.</t>
+  </si>
+  <si>
+    <t>Dado que se registra una transacción, el sistema guarda monto, fecha, y estado.
+Dado que el pago es exitoso, se genera un registro en Historial de pago.
+Dado que hay un error, se muestra mensaje y no cambia el estado.
+Dado que el administrador consulta, puede filtrar pagos por fecha y pasarela.</t>
+  </si>
+  <si>
+    <t>Dado que el cliente selecciona una pasarela activa, el sistema valida referencia de pago.
+Dado que el pago se procesa correctamente, se actualiza estado = pagado.
+Dado que el pago falla, se guarda detalle del error.
+Dado que se realiza un pago QR, el sistema permite cargar comprobante en imagen QR.</t>
+  </si>
+  <si>
+    <t>Dado que el administrador ingresa al módulo, ve registros ordenados por fecha.
+Dado que selecciona un pago, visualiza su detalle y referencia.
+Dado que exporta, el sistema genera archivo PDF o Excel.
+Dado que filtra por estado, se actualiza dinámicamente el listado.</t>
+  </si>
+  <si>
+    <t>Dado que el usuario navega entre módulos, las vistas cargan en menos de 2 segundos promedio.
+Dado que una vista supera ese tiempo, el sistema genera log de optimización.
+Dado que se ejecutan pruebas de rendimiento, el 95% cumple los tiempos esperados.</t>
+  </si>
+  <si>
+    <t>Dado que un usuario crea o cambia su contraseña, se aplica hash seguro.
+Dado que no cumple la política (mínimo 8 caracteres, mayúsculas, números, símbolo), se rechaza.
+Dado que se guarda una contraseña, nunca se almacena en texto plano.
+Dado que se audita el sistema, se verifica encriptación activa.</t>
   </si>
 </sst>
 </file>
@@ -376,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -398,6 +471,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162D0473-4A96-4D19-8D46-48218E926C7D}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="85" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="13.8"/>
@@ -801,7 +877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1">
+    <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -812,7 +888,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>13</v>
@@ -824,13 +900,13 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A4">
         <v>2</v>
       </c>
@@ -838,10 +914,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -853,13 +929,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A5">
         <v>3</v>
       </c>
@@ -867,10 +943,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -882,13 +958,13 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A6">
         <v>4</v>
       </c>
@@ -896,10 +972,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -911,13 +987,13 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A7">
         <v>5</v>
       </c>
@@ -925,10 +1001,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>13</v>
@@ -940,13 +1016,13 @@
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A8">
         <v>6</v>
       </c>
@@ -954,10 +1030,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -969,13 +1045,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A9">
         <v>7</v>
       </c>
@@ -983,10 +1059,10 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -998,13 +1074,13 @@
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1012,10 +1088,10 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1027,13 +1103,13 @@
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1041,10 +1117,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>13</v>
@@ -1053,16 +1129,16 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1070,10 +1146,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1082,16 +1158,16 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1099,10 +1175,10 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>5</v>
@@ -1111,16 +1187,16 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1128,10 +1204,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1140,16 +1216,16 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1157,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -1169,16 +1245,16 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
-      </c>
-      <c r="I15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1186,10 +1262,10 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1198,16 +1274,16 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1215,10 +1291,10 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1227,16 +1303,16 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1244,10 +1320,10 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1256,16 +1332,16 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
-      </c>
-      <c r="I18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1273,10 +1349,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19">
         <v>13</v>
@@ -1285,16 +1361,16 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
-      </c>
-      <c r="I19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1302,10 +1378,10 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20">
         <v>5</v>
@@ -1314,16 +1390,16 @@
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1331,10 +1407,10 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -1343,16 +1419,16 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1360,10 +1436,10 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1372,16 +1448,16 @@
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1389,10 +1465,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23">
         <v>8</v>
@@ -1401,16 +1477,16 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
-      </c>
-      <c r="I23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1418,10 +1494,10 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24">
         <v>5</v>
@@ -1430,16 +1506,16 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="H24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1447,10 +1523,10 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -1459,16 +1535,16 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="H25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="I25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1">
+    </row>
+    <row r="26" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1476,10 +1552,10 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -1488,16 +1564,16 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="40.049999999999997" customHeight="1">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1505,10 +1581,10 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27">
         <v>5</v>
@@ -1517,13 +1593,13 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>77</v>
-      </c>
-      <c r="I27" t="s">
-        <v>75</v>
+        <v>52</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>